<commit_message>
added dataProvider to BaseTest and updated excelsheet
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/actidata.xlsx
+++ b/src/test/resources/testdata/actidata.xlsx
@@ -1,18 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="usercredentials" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -342,12 +353,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>